<commit_message>
Adding LCS algorithm for mispelt or differently spelled workoutss
</commit_message>
<xml_diff>
--- a/Files/nutrition_workouts.xlsx
+++ b/Files/nutrition_workouts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6520" yWindow="3680" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6520" yWindow="3680" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="foods" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,6 @@
     <sheet name="diet" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="log" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="mood" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -21,19 +20,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-      <color rgb="FFBCBEC4"/>
-      <sz val="9.800000000000001"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,10 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +498,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -540,7 +532,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -581,10 +573,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -620,24 +612,6 @@
           <t>notes</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -712,54 +686,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="n">
-        <v>45761.59507233796</v>
-      </c>
-      <c r="B1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C1" t="n">
-        <v>9</v>
-      </c>
-      <c r="D1" t="n">
-        <v>9</v>
-      </c>
-      <c r="E1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G1" t="n">
-        <v>8</v>
-      </c>
-      <c r="H1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Called out. Feel really good today</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>